<commit_message>
renew bom for circuit
</commit_message>
<xml_diff>
--- a/manufacture/BOM_miniFOC.xlsx
+++ b/manufacture/BOM_miniFOC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Files\miniFOC\manufacture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C5C8A4-76BF-40BE-802B-4D3510421E4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2D6DD6-9094-4A64-8EB6-A461C3BD1461}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>100nF</t>
   </si>
@@ -43,9 +43,6 @@
     <t>C19702</t>
   </si>
   <si>
-    <t>C10,C11</t>
-  </si>
-  <si>
     <t>C0805</t>
   </si>
   <si>
@@ -213,10 +210,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>价格</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>数量</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -233,7 +226,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>合计金额</t>
+    <t>C10,C11,C14,C15</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>单价</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -583,7 +580,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -713,6 +710,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -842,14 +848,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1209,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1225,22 +1234,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1285,19 +1294,19 @@
     </row>
     <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F4" s="1">
         <v>8.6300000000000002E-2</v>
@@ -1305,19 +1314,19 @@
     </row>
     <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1">
         <v>4.1700000000000001E-2</v>
@@ -1325,19 +1334,19 @@
     </row>
     <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1">
         <v>1.0497000000000001</v>
@@ -1345,19 +1354,19 @@
     </row>
     <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1">
         <v>3.88</v>
@@ -1365,19 +1374,19 @@
     </row>
     <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1">
         <v>0.4294</v>
@@ -1385,19 +1394,19 @@
     </row>
     <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1">
         <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1">
         <v>0.14410000000000001</v>
@@ -1405,19 +1414,19 @@
     </row>
     <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1">
         <v>7.3000000000000001E-3</v>
@@ -1425,19 +1434,19 @@
     </row>
     <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1">
         <v>7.1999999999999998E-3</v>
@@ -1445,19 +1454,19 @@
     </row>
     <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="1">
         <v>8.0000000000000002E-3</v>
@@ -1465,19 +1474,19 @@
     </row>
     <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1">
         <v>5.0599999999999999E-2</v>
@@ -1485,19 +1494,19 @@
     </row>
     <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="1">
         <v>5.01</v>
@@ -1505,19 +1514,19 @@
     </row>
     <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="1">
         <v>1.95</v>
@@ -1525,19 +1534,19 @@
     </row>
     <row r="16" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="1">
         <v>0.16539999999999999</v>
@@ -1545,32 +1554,27 @@
     </row>
     <row r="17" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="1">
         <v>0.66539999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="1">
-        <f>SUM(F2:F17)</f>
-        <v>13.5672</v>
-      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
renew miniFOC PCB files and manufacture files
</commit_message>
<xml_diff>
--- a/manufacture/BOM_miniFOC.xlsx
+++ b/manufacture/BOM_miniFOC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Files\miniFOC\manufacture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2D6DD6-9094-4A64-8EB6-A461C3BD1461}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3380BFE3-D7E6-4D75-8367-6BB646C1597C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t>100nF</t>
   </si>
@@ -232,6 +232,20 @@
   <si>
     <t>单价</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>19-217/BHC-ZL1M2RY/3T</t>
+  </si>
+  <si>
+    <t>LED0603</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>C72041</t>
   </si>
 </sst>
 </file>
@@ -580,7 +594,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -710,15 +724,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -848,17 +853,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1218,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1573,8 +1575,24 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
+      <c r="A18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="1">
+        <v>9.8599999999999993E-2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>